<commit_message>
multi-BU support for supplier list: edge labels, supplier_id dedup, business_unit column
</commit_message>
<xml_diff>
--- a/templates/excel/omts-supplier-list-example.xlsx
+++ b/templates/excel/omts-supplier-list-example.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Supplier List" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Supplier List'!$A$4:$R$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Supplier List'!$A$4:$T$4</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -455,7 +455,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,22 +465,24 @@
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
     <col width="14" customWidth="1" min="2" max="2"/>
-    <col width="8" customWidth="1" min="3" max="3"/>
-    <col width="30" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="14" customWidth="1" min="6" max="6"/>
-    <col width="14" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
+    <col width="30" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
     <col width="14" customWidth="1" min="8" max="8"/>
-    <col width="16" customWidth="1" min="9" max="9"/>
-    <col width="24" customWidth="1" min="10" max="10"/>
-    <col width="14" customWidth="1" min="11" max="11"/>
-    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="14" customWidth="1" min="9" max="9"/>
+    <col width="14" customWidth="1" min="10" max="10"/>
+    <col width="16" customWidth="1" min="11" max="11"/>
+    <col width="24" customWidth="1" min="12" max="12"/>
     <col width="14" customWidth="1" min="13" max="13"/>
-    <col width="16" customWidth="1" min="14" max="14"/>
-    <col width="12" customWidth="1" min="15" max="15"/>
-    <col width="18" customWidth="1" min="16" max="16"/>
-    <col width="16" customWidth="1" min="17" max="17"/>
-    <col width="30" customWidth="1" min="18" max="18"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
+    <col width="14" customWidth="1" min="15" max="15"/>
+    <col width="16" customWidth="1" min="16" max="16"/>
+    <col width="12" customWidth="1" min="17" max="17"/>
+    <col width="18" customWidth="1" min="18" max="18"/>
+    <col width="16" customWidth="1" min="19" max="19"/>
+    <col width="30" customWidth="1" min="20" max="20"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -527,85 +529,95 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
+          <t>supplier_id</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
           <t>jurisdiction</t>
         </is>
       </c>
-      <c r="C4" s="4" t="inlineStr">
+      <c r="D4" s="4" t="inlineStr">
         <is>
           <t>tier</t>
         </is>
       </c>
-      <c r="D4" s="4" t="inlineStr">
+      <c r="E4" s="4" t="inlineStr">
         <is>
           <t>parent_supplier</t>
         </is>
       </c>
-      <c r="E4" s="4" t="inlineStr">
+      <c r="F4" s="4" t="inlineStr">
+        <is>
+          <t>business_unit</t>
+        </is>
+      </c>
+      <c r="G4" s="4" t="inlineStr">
         <is>
           <t>commodity</t>
         </is>
       </c>
-      <c r="F4" s="4" t="inlineStr">
+      <c r="H4" s="4" t="inlineStr">
         <is>
           <t>valid_from</t>
         </is>
       </c>
-      <c r="G4" s="4" t="inlineStr">
+      <c r="I4" s="4" t="inlineStr">
         <is>
           <t>annual_value</t>
         </is>
       </c>
-      <c r="H4" s="4" t="inlineStr">
+      <c r="J4" s="4" t="inlineStr">
         <is>
           <t>value_currency</t>
         </is>
       </c>
-      <c r="I4" s="4" t="inlineStr">
+      <c r="K4" s="4" t="inlineStr">
         <is>
           <t>contract_ref</t>
         </is>
       </c>
-      <c r="J4" s="4" t="inlineStr">
+      <c r="L4" s="4" t="inlineStr">
         <is>
           <t>lei</t>
         </is>
       </c>
-      <c r="K4" s="4" t="inlineStr">
+      <c r="M4" s="4" t="inlineStr">
         <is>
           <t>duns</t>
         </is>
       </c>
-      <c r="L4" s="4" t="inlineStr">
+      <c r="N4" s="4" t="inlineStr">
         <is>
           <t>vat</t>
         </is>
       </c>
-      <c r="M4" s="4" t="inlineStr">
+      <c r="O4" s="4" t="inlineStr">
         <is>
           <t>vat_country</t>
         </is>
       </c>
-      <c r="N4" s="4" t="inlineStr">
+      <c r="P4" s="4" t="inlineStr">
         <is>
           <t>internal_id</t>
         </is>
       </c>
-      <c r="O4" s="4" t="inlineStr">
+      <c r="Q4" s="4" t="inlineStr">
         <is>
           <t>risk_tier</t>
         </is>
       </c>
-      <c r="P4" s="4" t="inlineStr">
+      <c r="R4" s="4" t="inlineStr">
         <is>
           <t>kraljic_quadrant</t>
         </is>
       </c>
-      <c r="Q4" s="4" t="inlineStr">
+      <c r="S4" s="4" t="inlineStr">
         <is>
           <t>approval_status</t>
         </is>
       </c>
-      <c r="R4" s="4" t="inlineStr">
+      <c r="T4" s="4" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
@@ -619,51 +631,61 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>bolt-001</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>GB</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>1</v>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Procurement</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>7318.15</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>2023-01-15</t>
         </is>
       </c>
-      <c r="G5" t="n">
+      <c r="I5" t="n">
         <v>450000</v>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>EUR</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>MSA-2023-001</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>234567890</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>low</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="R5" t="inlineStr">
         <is>
           <t>strategic</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="S5" t="inlineStr">
         <is>
           <t>approved</t>
         </is>
@@ -675,48 +697,53 @@
           <t>Nordic Fasteners AB</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>SE</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>1</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Procurement</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>7318.15</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>2024-06-01</t>
         </is>
       </c>
-      <c r="G6" t="n">
+      <c r="I6" t="n">
         <v>120000</v>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>EUR</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>medium</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="R6" t="inlineStr">
         <is>
           <t>leverage</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
+      <c r="S6" t="inlineStr">
         <is>
           <t>conditional</t>
         </is>
       </c>
-      <c r="R6" t="inlineStr">
+      <c r="T6" t="inlineStr">
         <is>
           <t>Under evaluation; trial order in progress</t>
         </is>
@@ -730,51 +757,61 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>shan-001</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>CN</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>1</v>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Procurement</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>7228.70</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>2022-03-01</t>
         </is>
       </c>
-      <c r="G7" t="n">
+      <c r="I7" t="n">
         <v>800000</v>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>FWA-2022-008</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>V-200891</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
+      <c r="Q7" t="inlineStr">
         <is>
           <t>high</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
+      <c r="R7" t="inlineStr">
         <is>
           <t>bottleneck</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr">
+      <c r="S7" t="inlineStr">
         <is>
           <t>approved</t>
         </is>
@@ -783,38 +820,56 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Yorkshire Steel Works</t>
+          <t>Bolt Supplies Ltd</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>bolt-001</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>GB</t>
         </is>
       </c>
-      <c r="C8" t="n">
-        <v>2</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Bolt Supplies Ltd</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>7208.10</t>
-        </is>
+      <c r="D8" t="n">
+        <v>1</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2021-09-01</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>low</t>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>7318.16</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>180000</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>EUR</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>non-critical</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
         <is>
           <t>approved</t>
         </is>
@@ -823,94 +878,134 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Baosteel Trading Co</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
+          <t>Yorkshire Steel Works</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
         <v>2</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Shanghai Steel Components Co</t>
-        </is>
-      </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>7207.11</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>2020-01-15</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>high</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>Primary raw material supplier for Shanghai Steel</t>
+          <t>bolt-001</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>7208.10</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2021-09-01</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>approved</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>Baosteel Trading Co</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>shan-001</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>7207.11</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2020-01-15</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>high</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>Primary raw material supplier for Shanghai Steel</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>Inner Mongolia Mining Corp</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>CN</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="D11" t="n">
         <v>3</v>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>Baosteel Trading Co</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>2601.11</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="Q11" t="inlineStr">
         <is>
           <t>critical</t>
         </is>
       </c>
-      <c r="R10" t="inlineStr">
+      <c r="T11" t="inlineStr">
         <is>
           <t>Iron ore source; LKSG high-risk region</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:R4"/>
+  <autoFilter ref="A4:T4"/>
   <dataValidations count="5">
     <dataValidation sqref="B2" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="1" promptTitle="Disclosure Scope" prompt="Who will see this file? (default: partner)" type="list">
       <formula1>"internal,partner,public"</formula1>
     </dataValidation>
-    <dataValidation sqref="C5:C10000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" promptTitle="Tier" prompt="Supply-chain tier: 1 = direct, 2 = sub-supplier, 3 = sub-sub-supplier" type="list">
+    <dataValidation sqref="D5:D10000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" promptTitle="Tier" prompt="Supply-chain tier: 1 = direct, 2 = sub-supplier, 3 = sub-sub-supplier" type="list">
       <formula1>"1,2,3"</formula1>
     </dataValidation>
-    <dataValidation sqref="O5:O10000" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="1" promptTitle="Risk Tier" prompt="General risk classification" type="list">
+    <dataValidation sqref="Q5:Q10000" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="1" promptTitle="Risk Tier" prompt="General risk classification" type="list">
       <formula1>"critical,high,medium,low"</formula1>
     </dataValidation>
-    <dataValidation sqref="P5:P10000" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="1" promptTitle="Kraljic Quadrant" prompt="Kraljic portfolio classification" type="list">
+    <dataValidation sqref="R5:R10000" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="1" promptTitle="Kraljic Quadrant" prompt="Kraljic portfolio classification" type="list">
       <formula1>"strategic,leverage,bottleneck,non-critical"</formula1>
     </dataValidation>
-    <dataValidation sqref="Q5:Q10000" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="1" promptTitle="Approval Status" prompt="Supplier approval status" type="list">
+    <dataValidation sqref="S5:S10000" showDropDown="0" showInputMessage="1" showErrorMessage="0" allowBlank="1" promptTitle="Approval Status" prompt="Supplier approval status" type="list">
       <formula1>"approved,conditional,pending,blocked,phase-out"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>